<commit_message>
Added changes to screen-authorization.xlxs
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/screen_authorization.xlsx
+++ b/mosip_master/xlsx/screen_authorization.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1044292\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,68 +24,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
-  <si>
-    <t xml:space="preserve">lang_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">screen_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role_code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_permitted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">is_active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eodRoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTRATION_SUPERVISOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTRATION_ADMIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reRegisterRoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lostUINRoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REGISTRATION_OFFICER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newRegistrationRoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reportRoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uinUpdateRoot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uploadPacketRoot</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="18">
+  <si>
+    <t>lang_code</t>
+  </si>
+  <si>
+    <t>screen_id</t>
+  </si>
+  <si>
+    <t>role_code</t>
+  </si>
+  <si>
+    <t>is_permitted</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>eodRoot</t>
+  </si>
+  <si>
+    <t>REGISTRATION_SUPERVISOR</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>REGISTRATION_ADMIN</t>
+  </si>
+  <si>
+    <t>reRegisterRoot</t>
+  </si>
+  <si>
+    <t>lostUINRoot</t>
+  </si>
+  <si>
+    <t>REGISTRATION_OFFICER</t>
+  </si>
+  <si>
+    <t>newRegistrationRoot</t>
+  </si>
+  <si>
+    <t>reportRoot</t>
+  </si>
+  <si>
+    <t>uinUpdateRoot</t>
+  </si>
+  <si>
+    <t>uploadPacketRoot</t>
+  </si>
+  <si>
+    <t>correctionRoot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -90,25 +93,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -121,96 +108,366 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="8.43"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -227,7 +484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -244,7 +501,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -261,7 +518,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -278,7 +535,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -295,7 +552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -312,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -329,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -346,7 +603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -363,7 +620,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -380,7 +637,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -397,7 +654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -414,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -431,7 +688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -448,7 +705,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
@@ -465,7 +722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -482,7 +739,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
@@ -499,7 +756,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -516,7 +773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
@@ -533,13 +790,59 @@
         <v>8</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>